<commit_message>
update the correct version for boundary
</commit_message>
<xml_diff>
--- a/experiment1_analysis/stimuliid_boundaries.xlsx
+++ b/experiment1_analysis/stimuliid_boundaries.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Eye_Tracking_Education_Video\experiment1_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1758712C-365C-436F-8952-15FA7B5BB9D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9857D4C2-989F-40C8-A038-A34C6CA39736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4584" yWindow="3348" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -853,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" workbookViewId="0">
-      <selection activeCell="H137" sqref="H137"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -887,10 +887,10 @@
         <v>1280</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E2">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -904,10 +904,10 @@
         <v>1280</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E3">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -921,10 +921,10 @@
         <v>1280</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E4">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -938,10 +938,10 @@
         <v>1280</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E5">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -955,10 +955,10 @@
         <v>1280</v>
       </c>
       <c r="D6">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E6">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -972,10 +972,10 @@
         <v>1280</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E7">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -989,10 +989,10 @@
         <v>1280</v>
       </c>
       <c r="D8">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E8">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1006,10 +1006,10 @@
         <v>1280</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E9">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -1023,10 +1023,10 @@
         <v>1280</v>
       </c>
       <c r="D10">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E10">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -1040,10 +1040,10 @@
         <v>1280</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E11">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1057,10 +1057,10 @@
         <v>1280</v>
       </c>
       <c r="D12">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E12">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1074,10 +1074,10 @@
         <v>1280</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E13">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1091,10 +1091,10 @@
         <v>1280</v>
       </c>
       <c r="D14">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E14">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1108,10 +1108,10 @@
         <v>1280</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E15">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1125,10 +1125,10 @@
         <v>1280</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E16">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1142,10 +1142,10 @@
         <v>1280</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E17">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1159,10 +1159,10 @@
         <v>1280</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E18">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1176,10 +1176,10 @@
         <v>1280</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E19">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="20" spans="1:5">
@@ -1193,10 +1193,10 @@
         <v>1280</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E20">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1210,10 +1210,10 @@
         <v>1280</v>
       </c>
       <c r="D21">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E21">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -1227,10 +1227,10 @@
         <v>1280</v>
       </c>
       <c r="D22">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E22">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -1244,10 +1244,10 @@
         <v>1280</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E23">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1261,10 +1261,10 @@
         <v>1280</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E24">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1278,10 +1278,10 @@
         <v>1280</v>
       </c>
       <c r="D25">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E25">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1295,10 +1295,10 @@
         <v>1280</v>
       </c>
       <c r="D26">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E26">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -1312,10 +1312,10 @@
         <v>1280</v>
       </c>
       <c r="D27">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E27">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="28" spans="1:5">
@@ -1329,10 +1329,10 @@
         <v>1280</v>
       </c>
       <c r="D28">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E28">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1346,10 +1346,10 @@
         <v>1280</v>
       </c>
       <c r="D29">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E29">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="30" spans="1:5">
@@ -1363,10 +1363,10 @@
         <v>1280</v>
       </c>
       <c r="D30">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E30">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -1380,10 +1380,10 @@
         <v>1280</v>
       </c>
       <c r="D31">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E31">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -1397,10 +1397,10 @@
         <v>1280</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E32">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1414,10 +1414,10 @@
         <v>1280</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E33">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1431,10 +1431,10 @@
         <v>1280</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E34">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="35" spans="1:5">
@@ -1448,10 +1448,10 @@
         <v>1280</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E35">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1465,10 +1465,10 @@
         <v>1280</v>
       </c>
       <c r="D36">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E36">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1482,10 +1482,10 @@
         <v>1280</v>
       </c>
       <c r="D37">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E37">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1499,10 +1499,10 @@
         <v>1280</v>
       </c>
       <c r="D38">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E38">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="39" spans="1:5">
@@ -1516,10 +1516,10 @@
         <v>1280</v>
       </c>
       <c r="D39">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E39">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -1533,10 +1533,10 @@
         <v>1280</v>
       </c>
       <c r="D40">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E40">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -1550,10 +1550,10 @@
         <v>1280</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E41">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -1567,10 +1567,10 @@
         <v>1280</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E42">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="43" spans="1:5">
@@ -1584,10 +1584,10 @@
         <v>1280</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E43">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -1601,10 +1601,10 @@
         <v>1280</v>
       </c>
       <c r="D44">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E44">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -1618,10 +1618,10 @@
         <v>1280</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E45">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -1635,10 +1635,10 @@
         <v>1280</v>
       </c>
       <c r="D46">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E46">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -1652,10 +1652,10 @@
         <v>1280</v>
       </c>
       <c r="D47">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E47">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="48" spans="1:5">
@@ -1669,10 +1669,10 @@
         <v>1280</v>
       </c>
       <c r="D48">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E48">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -1686,10 +1686,10 @@
         <v>1280</v>
       </c>
       <c r="D49">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E49">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -1703,10 +1703,10 @@
         <v>1280</v>
       </c>
       <c r="D50">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E50">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -1720,10 +1720,10 @@
         <v>1280</v>
       </c>
       <c r="D51">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E51">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -1737,10 +1737,10 @@
         <v>1280</v>
       </c>
       <c r="D52">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E52">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -1754,10 +1754,10 @@
         <v>1280</v>
       </c>
       <c r="D53">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E53">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -1771,10 +1771,10 @@
         <v>1280</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E54">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -1788,10 +1788,10 @@
         <v>1280</v>
       </c>
       <c r="D55">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E55">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -1805,10 +1805,10 @@
         <v>1280</v>
       </c>
       <c r="D56">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E56">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="57" spans="1:5">
@@ -1822,10 +1822,10 @@
         <v>1280</v>
       </c>
       <c r="D57">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E57">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -1839,10 +1839,10 @@
         <v>1280</v>
       </c>
       <c r="D58">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E58">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="59" spans="1:5">
@@ -1856,10 +1856,10 @@
         <v>1280</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E59">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -1873,10 +1873,10 @@
         <v>1280</v>
       </c>
       <c r="D60">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E60">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -1890,10 +1890,10 @@
         <v>1280</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E61">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -1907,10 +1907,10 @@
         <v>1280</v>
       </c>
       <c r="D62">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E62">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -1924,10 +1924,10 @@
         <v>1280</v>
       </c>
       <c r="D63">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E63">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="64" spans="1:5">
@@ -1941,10 +1941,10 @@
         <v>1280</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E64">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -1958,10 +1958,10 @@
         <v>1280</v>
       </c>
       <c r="D65">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E65">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="66" spans="1:5">
@@ -1975,10 +1975,10 @@
         <v>1280</v>
       </c>
       <c r="D66">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E66">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -1992,10 +1992,10 @@
         <v>1280</v>
       </c>
       <c r="D67">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E67">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -2009,10 +2009,10 @@
         <v>1280</v>
       </c>
       <c r="D68">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E68">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -2026,10 +2026,10 @@
         <v>1280</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E69">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2043,10 +2043,10 @@
         <v>1280</v>
       </c>
       <c r="D70">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E70">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="71" spans="1:5">
@@ -2060,10 +2060,10 @@
         <v>1280</v>
       </c>
       <c r="D71">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E71">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -2077,10 +2077,10 @@
         <v>1280</v>
       </c>
       <c r="D72">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E72">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -2094,10 +2094,10 @@
         <v>1280</v>
       </c>
       <c r="D73">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E73">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2111,10 +2111,10 @@
         <v>1280</v>
       </c>
       <c r="D74">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E74">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2128,10 +2128,10 @@
         <v>1280</v>
       </c>
       <c r="D75">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E75">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -2145,10 +2145,10 @@
         <v>1280</v>
       </c>
       <c r="D76">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E76">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2162,10 +2162,10 @@
         <v>1280</v>
       </c>
       <c r="D77">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E77">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="78" spans="1:5">
@@ -2179,10 +2179,10 @@
         <v>1280</v>
       </c>
       <c r="D78">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E78">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="79" spans="1:5">
@@ -2196,10 +2196,10 @@
         <v>1280</v>
       </c>
       <c r="D79">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E79">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2213,10 +2213,10 @@
         <v>1280</v>
       </c>
       <c r="D80">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E80">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -2230,10 +2230,10 @@
         <v>1280</v>
       </c>
       <c r="D81">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E81">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -2247,10 +2247,10 @@
         <v>1280</v>
       </c>
       <c r="D82">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E82">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2264,10 +2264,10 @@
         <v>1280</v>
       </c>
       <c r="D83">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E83">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2281,10 +2281,10 @@
         <v>1280</v>
       </c>
       <c r="D84">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E84">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -2298,10 +2298,10 @@
         <v>1280</v>
       </c>
       <c r="D85">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E85">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -2315,10 +2315,10 @@
         <v>1280</v>
       </c>
       <c r="D86">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E86">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -2332,10 +2332,10 @@
         <v>1280</v>
       </c>
       <c r="D87">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E87">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -2349,10 +2349,10 @@
         <v>1280</v>
       </c>
       <c r="D88">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E88">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2366,10 +2366,10 @@
         <v>1280</v>
       </c>
       <c r="D89">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E89">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -2383,10 +2383,10 @@
         <v>1280</v>
       </c>
       <c r="D90">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E90">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="91" spans="1:5">
@@ -2400,10 +2400,10 @@
         <v>1280</v>
       </c>
       <c r="D91">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E91">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="92" spans="1:5">
@@ -2417,10 +2417,10 @@
         <v>1280</v>
       </c>
       <c r="D92">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E92">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2434,10 +2434,10 @@
         <v>1280</v>
       </c>
       <c r="D93">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E93">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2451,10 +2451,10 @@
         <v>1280</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E94">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="95" spans="1:5">
@@ -2468,10 +2468,10 @@
         <v>1280</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E95">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -2485,10 +2485,10 @@
         <v>1280</v>
       </c>
       <c r="D96">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E96">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2502,10 +2502,10 @@
         <v>1280</v>
       </c>
       <c r="D97">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E97">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2519,10 +2519,10 @@
         <v>1280</v>
       </c>
       <c r="D98">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E98">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2536,10 +2536,10 @@
         <v>1280</v>
       </c>
       <c r="D99">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E99">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -2553,10 +2553,10 @@
         <v>1280</v>
       </c>
       <c r="D100">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E100">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="101" spans="1:5">
@@ -2570,10 +2570,10 @@
         <v>1280</v>
       </c>
       <c r="D101">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E101">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -2587,10 +2587,10 @@
         <v>1280</v>
       </c>
       <c r="D102">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E102">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -2604,10 +2604,10 @@
         <v>1280</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E103">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -2621,10 +2621,10 @@
         <v>1280</v>
       </c>
       <c r="D104">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E104">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -2638,10 +2638,10 @@
         <v>1280</v>
       </c>
       <c r="D105">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E105">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="106" spans="1:5">
@@ -2655,10 +2655,10 @@
         <v>1280</v>
       </c>
       <c r="D106">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E106">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="107" spans="1:5">
@@ -2672,10 +2672,10 @@
         <v>1280</v>
       </c>
       <c r="D107">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E107">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="108" spans="1:5">
@@ -2689,10 +2689,10 @@
         <v>1280</v>
       </c>
       <c r="D108">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E108">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -2706,10 +2706,10 @@
         <v>1280</v>
       </c>
       <c r="D109">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E109">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="110" spans="1:5">
@@ -2723,10 +2723,10 @@
         <v>1280</v>
       </c>
       <c r="D110">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E110">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -2740,10 +2740,10 @@
         <v>1280</v>
       </c>
       <c r="D111">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E111">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -2757,10 +2757,10 @@
         <v>1280</v>
       </c>
       <c r="D112">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E112">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -2774,10 +2774,10 @@
         <v>1280</v>
       </c>
       <c r="D113">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E113">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="114" spans="1:5">
@@ -2791,10 +2791,10 @@
         <v>1280</v>
       </c>
       <c r="D114">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E114">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="115" spans="1:5">
@@ -2808,10 +2808,10 @@
         <v>1280</v>
       </c>
       <c r="D115">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E115">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="116" spans="1:5">
@@ -2825,10 +2825,10 @@
         <v>1280</v>
       </c>
       <c r="D116">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E116">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -2842,10 +2842,10 @@
         <v>1280</v>
       </c>
       <c r="D117">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E117">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -2859,10 +2859,10 @@
         <v>1280</v>
       </c>
       <c r="D118">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E118">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -2876,10 +2876,10 @@
         <v>1280</v>
       </c>
       <c r="D119">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E119">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -2893,10 +2893,10 @@
         <v>1280</v>
       </c>
       <c r="D120">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E120">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -2910,10 +2910,10 @@
         <v>1280</v>
       </c>
       <c r="D121">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E121">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -2927,10 +2927,10 @@
         <v>1280</v>
       </c>
       <c r="D122">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E122">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -2944,10 +2944,10 @@
         <v>1280</v>
       </c>
       <c r="D123">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E123">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -2961,10 +2961,10 @@
         <v>1280</v>
       </c>
       <c r="D124">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E124">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="125" spans="1:5">
@@ -2978,10 +2978,10 @@
         <v>1280</v>
       </c>
       <c r="D125">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E125">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="126" spans="1:5">
@@ -2995,10 +2995,10 @@
         <v>1280</v>
       </c>
       <c r="D126">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E126">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -3012,10 +3012,10 @@
         <v>1280</v>
       </c>
       <c r="D127">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E127">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3029,10 +3029,10 @@
         <v>1280</v>
       </c>
       <c r="D128">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E128">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3046,10 +3046,10 @@
         <v>1280</v>
       </c>
       <c r="D129">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E129">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -3063,10 +3063,10 @@
         <v>1280</v>
       </c>
       <c r="D130">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E130">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -3080,10 +3080,10 @@
         <v>1280</v>
       </c>
       <c r="D131">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E131">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -3097,10 +3097,10 @@
         <v>1280</v>
       </c>
       <c r="D132">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E132">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="133" spans="1:5">
@@ -3114,10 +3114,10 @@
         <v>1280</v>
       </c>
       <c r="D133">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E133">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -3131,10 +3131,10 @@
         <v>1280</v>
       </c>
       <c r="D134">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E134">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -3148,10 +3148,10 @@
         <v>1280</v>
       </c>
       <c r="D135">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E135">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3165,10 +3165,10 @@
         <v>1280</v>
       </c>
       <c r="D136">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E136">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="137" spans="1:5">
@@ -3182,10 +3182,10 @@
         <v>1280</v>
       </c>
       <c r="D137">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E137">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3199,10 +3199,10 @@
         <v>1280</v>
       </c>
       <c r="D138">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E138">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3216,10 +3216,10 @@
         <v>1280</v>
       </c>
       <c r="D139">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E139">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -3233,10 +3233,10 @@
         <v>1280</v>
       </c>
       <c r="D140">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E140">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3250,10 +3250,10 @@
         <v>1280</v>
       </c>
       <c r="D141">
-        <v>1</v>
+        <v>153</v>
       </c>
       <c r="E141">
-        <v>720</v>
+        <v>872</v>
       </c>
     </row>
   </sheetData>

</xml_diff>